<commit_message>
Revert "Allow for postman"
This reverts commit 4329471e26311ad2d9ce1afeec6c323401589415.
</commit_message>
<xml_diff>
--- a/manual-tests/manual-tests.xlsx
+++ b/manual-tests/manual-tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://simonyi-my.sharepoint.com/personal/fendre8_sch_bme_hu/Documents/BME/6. félév/IET/házi/hf2/iet-hf2021-todo-team-name/manual-tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{236D6BF3-98C6-4993-8BE3-2E26933D8511}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{49E82AD6-27A8-4B24-8C59-0E6E55418E1F}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{236D6BF3-98C6-4993-8BE3-2E26933D8511}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0A4375A0-E268-412F-B2CF-45752DEB75C7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{2C77ACA4-CDF2-465F-BF8B-0D5028445B99}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{2C77ACA4-CDF2-465F-BF8B-0D5028445B99}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontend" sheetId="1" r:id="rId1"/>
@@ -1164,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{918DC292-13A7-4F29-AA3E-C37D7E31DB13}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Revert "Revert "Allow for postman""
This reverts commit 9059bfd3d9ea02727f699e48b5ddb0340ea19507.
</commit_message>
<xml_diff>
--- a/manual-tests/manual-tests.xlsx
+++ b/manual-tests/manual-tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://simonyi-my.sharepoint.com/personal/fendre8_sch_bme_hu/Documents/BME/6. félév/IET/házi/hf2/iet-hf2021-todo-team-name/manual-tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{236D6BF3-98C6-4993-8BE3-2E26933D8511}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0A4375A0-E268-412F-B2CF-45752DEB75C7}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{236D6BF3-98C6-4993-8BE3-2E26933D8511}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{49E82AD6-27A8-4B24-8C59-0E6E55418E1F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{2C77ACA4-CDF2-465F-BF8B-0D5028445B99}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{2C77ACA4-CDF2-465F-BF8B-0D5028445B99}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontend" sheetId="1" r:id="rId1"/>
@@ -1164,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{918DC292-13A7-4F29-AA3E-C37D7E31DB13}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>